<commit_message>
fix : updated sheets
</commit_message>
<xml_diff>
--- a/NBFC.xlsx
+++ b/NBFC.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="155">
   <si>
     <t>NBFC</t>
   </si>
@@ -91,13 +91,13 @@
     <t xml:space="preserve">CRAR  (capital adequacy)</t>
   </si>
   <si>
-    <t xml:space="preserve">How's strong is the company's own capital compared to the risks it takes </t>
+    <t xml:space="preserve">How's strong is the company's own capital compared to the risks it takes ( own assets [that include equity + prev profits] / weighted debt [weighted based on the riskiness]) </t>
   </si>
   <si>
     <t xml:space="preserve">Tier-1 capital </t>
   </si>
   <si>
-    <t xml:space="preserve">High-quality own money  (equity , profits, reinvestments) </t>
+    <t xml:space="preserve">High-quality own money  (equity , profits, reinvestments)  , this is represented in terms of % to the total debt raised </t>
   </si>
   <si>
     <t xml:space="preserve">Tier-2 capital </t>
@@ -118,6 +118,24 @@
     <t xml:space="preserve">Directly to individual, consumers for personal use </t>
   </si>
   <si>
+    <t xml:space="preserve">Provision Coverage Ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How much NPA / bad-debts are covered from provision funds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standard Asset Coverage Ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Own money / good loans </t>
+  </si>
+  <si>
+    <t xml:space="preserve">weighted average no of shares </t>
+  </si>
+  <si>
+    <t xml:space="preserve">lets suppose for first six months company had 1,00,000 shares and in the next 6 months they released 50,000 more shares ... so when we calculate total no of shares in a year it would be (12*1,00,000  +  6*50,000) / 12 , no. of shares </t>
+  </si>
+  <si>
     <t>LIST</t>
   </si>
   <si>
@@ -128,6 +146,18 @@
   </si>
   <si>
     <t xml:space="preserve">Jio financial serviced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cholamandalam investment and finance company limited</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Muthoot finance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shriram finance </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mahindra finance</t>
   </si>
   <si>
     <t xml:space="preserve">Bajaj finance</t>
@@ -465,12 +495,17 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* &quot;(&quot;#,##0&quot;)&quot;;_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11.000000"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10.000000"/>
+      <color theme="1"/>
+      <name val="Rubik"/>
     </font>
     <font>
       <u/>
@@ -507,12 +542,10 @@
     <font>
       <b/>
       <sz val="12.000000"/>
-      <color indexed="64"/>
       <name val="Arial"/>
     </font>
     <font>
       <sz val="12.000000"/>
-      <color indexed="64"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -527,12 +560,27 @@
       <patternFill patternType="none"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left style="none"/>
       <right style="none"/>
       <top style="none"/>
       <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal style="none"/>
     </border>
     <border>
@@ -555,7 +603,7 @@
         <color rgb="FFCCCCCC"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
         <color rgb="FFCCCCCC"/>
@@ -571,27 +619,28 @@
     <xf fontId="0" fillId="2" borderId="0" numFmtId="43" applyNumberFormat="1" applyFont="0" applyFill="0" applyBorder="0"/>
     <xf fontId="0" fillId="2" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="0" applyFill="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="164" xfId="1" applyNumberFormat="1"/>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="164" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="164" xfId="1" applyNumberFormat="1" applyFont="1">
+    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="3" fillId="0" borderId="0" numFmtId="164" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf fontId="3" fillId="0" borderId="0" numFmtId="164" xfId="1" applyNumberFormat="1" applyFont="1">
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="164" xfId="1" applyNumberFormat="1">
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="9" xfId="2" applyNumberFormat="1"/>
-    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="3" fillId="0" borderId="0" numFmtId="165" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf fontId="3" fillId="0" borderId="0" numFmtId="165" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf fontId="3" fillId="0" borderId="0" numFmtId="164" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf fontId="5" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="4" fillId="0" borderId="0" numFmtId="165" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf fontId="4" fillId="0" borderId="0" numFmtId="165" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf fontId="4" fillId="0" borderId="0" numFmtId="164" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="5" fillId="0" borderId="0" numFmtId="164" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="9" xfId="2" applyNumberFormat="1">
       <protection hidden="0" locked="1"/>
     </xf>
@@ -599,25 +648,25 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="3" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="4" fillId="0" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf fontId="5" fillId="0" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="6" fillId="0" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf fontId="3" fillId="0" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf fontId="6" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="4" fillId="0" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf fontId="7" fillId="0" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf fontId="7" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="8" fillId="0" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf fontId="7" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="8" fillId="0" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf fontId="8" fillId="0" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -644,11 +693,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>573881</xdr:colOff>
+      <xdr:colOff>573880</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="7879535" cy="4438649"/>
+    <xdr:ext cx="7879535" cy="4438648"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="1493204001" name=""/>
@@ -1168,13 +1217,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A24" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="18.00390625"/>
+    <col customWidth="1" min="2" max="2" width="29.421875"/>
     <col customWidth="1" min="3" max="3" width="19.57421875"/>
   </cols>
   <sheetData>
@@ -1298,58 +1347,101 @@
         <v>27</v>
       </c>
     </row>
+    <row r="20">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+    </row>
     <row r="21">
-      <c r="B21" t="s">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23"/>
+    <row r="24">
+      <c r="B24" t="s">
         <v>28</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C24" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="22">
-      <c r="B22" s="1" t="s">
+    <row r="25">
+      <c r="B25" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="23">
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-    </row>
-    <row r="24">
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-    </row>
-    <row r="25">
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-    </row>
-    <row r="26"/>
+    <row r="26">
+      <c r="B26" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
     <row r="27">
-      <c r="B27" t="s">
-        <v>32</v>
+      <c r="B27" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="28">
-      <c r="C28" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="C29" t="s">
-        <v>34</v>
+      <c r="B28" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="30">
-      <c r="C30" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="C43"/>
-    </row>
+      <c r="B30" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="C31" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="C32" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="C33" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" ht="14.25">
+      <c r="C34" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" ht="14.25">
+      <c r="C35" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" ht="14.25">
+      <c r="C36" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37" ht="14.25">
+      <c r="C37" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="43"/>
+    <row r="46"/>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
@@ -1375,557 +1467,557 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>37</v>
+        <v>46</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="2">
       <c r="C2" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="D2" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="E2" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="F2" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="G2" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="H2" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="I2" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="J2" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3" s="3">
+        <v>56</v>
+      </c>
+      <c r="C3" s="5">
         <v>15.300000000000001</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="5">
         <v>23.5</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="5">
         <v>27.399999999999999</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="5">
         <v>16.899999999999999</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="5">
         <v>24.699999999999999</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="5">
         <v>29.600000000000001</v>
       </c>
-      <c r="I3" s="3">
+      <c r="I3" s="5">
         <v>36.200000000000003</v>
       </c>
-      <c r="J3" s="3">
+      <c r="J3" s="5">
         <v>43.399999999999999</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" s="3">
+        <v>57</v>
+      </c>
+      <c r="C4" s="5">
         <v>82400</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="5">
         <v>115900</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="5">
         <v>147200</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="5">
         <v>152900</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="5">
         <v>197500</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="5">
         <v>247400</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="5">
         <v>330600</v>
       </c>
-      <c r="J4" s="3">
+      <c r="J4" s="5">
         <v>416700</v>
       </c>
     </row>
-    <row r="5" s="4" customFormat="1">
-      <c r="B5" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C5" s="5">
+    <row r="5" s="6" customFormat="1">
+      <c r="B5" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="7">
         <v>12757</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="7">
         <v>18500</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="7">
         <v>26386</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="7">
         <v>26683</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="7">
         <v>31648</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="7">
         <v>41418</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="7">
         <v>54983</v>
       </c>
-      <c r="J5" s="5">
+      <c r="J5" s="7">
         <v>69725</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" s="3">
+        <v>59</v>
+      </c>
+      <c r="C6" s="5">
         <v>4614</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="5">
         <v>6623</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="5">
         <v>9473</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="5">
         <v>9414</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="5">
         <v>9754</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="5">
         <v>12560</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="5">
         <v>18725</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6" s="5">
         <v>24771</v>
       </c>
     </row>
-    <row r="7" s="4" customFormat="1">
-      <c r="A7" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C7" s="5">
+    <row r="7" s="6" customFormat="1">
+      <c r="A7" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" s="7">
         <f>C5-C6</f>
         <v>8143</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="7">
         <f>D5-D6</f>
         <v>11877</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="7">
         <f>E5-E6</f>
         <v>16913</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="7">
         <f>F5-F6</f>
         <v>17269</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="7">
         <f>G5-G6</f>
         <v>21894</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="7">
         <f>H5-H6</f>
         <v>28858</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I7" s="7">
         <f>I5-I6</f>
         <v>36258</v>
       </c>
-      <c r="J7" s="5">
+      <c r="J7" s="7">
         <f>J5-J6</f>
         <v>44954</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C8" s="3">
+        <v>62</v>
+      </c>
+      <c r="C8" s="5">
         <v>3270</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="5">
         <v>4197</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="5">
         <v>5662</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="5">
         <v>5308</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="5">
         <v>7587</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="5">
         <v>10142</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I8" s="5">
         <v>12325</v>
       </c>
-      <c r="J8" s="3">
+      <c r="J8" s="5">
         <v>14926</v>
       </c>
     </row>
-    <row r="9" s="4" customFormat="1">
-      <c r="B9" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C9" s="5">
+    <row r="9" s="6" customFormat="1">
+      <c r="B9" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="7">
         <f>C7-C8</f>
         <v>4873</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="8">
         <f>D7-D8</f>
         <v>7680</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="8">
         <f>E7-E8</f>
         <v>11251</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="8">
         <f>F7-F8</f>
         <v>11961</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="8">
         <f>G7-G8</f>
         <v>14307</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="8">
         <f>H7-H8</f>
         <v>18716</v>
       </c>
-      <c r="I9" s="6">
+      <c r="I9" s="8">
         <f>I7-I8</f>
         <v>23933</v>
       </c>
-      <c r="J9" s="6">
+      <c r="J9" s="8">
         <f>J7-J8</f>
         <v>30028</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="B10" t="s">
-        <v>55</v>
-      </c>
-      <c r="C10" s="3">
+        <v>65</v>
+      </c>
+      <c r="C10" s="5">
         <v>1030</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="5">
         <v>1501</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="5">
         <v>3929</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="5">
         <v>5969</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="5">
         <v>4803</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="5">
         <v>3190</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I10" s="5">
         <v>4631</v>
       </c>
-      <c r="J10" s="3">
+      <c r="J10" s="5">
         <v>7966</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" t="s">
-        <v>56</v>
-      </c>
-      <c r="C11" s="3">
+        <v>66</v>
+      </c>
+      <c r="C11" s="5">
         <f>C9-C10</f>
         <v>3843</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="9">
         <f>D9-D10</f>
         <v>6179</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="9">
         <f>E9-E10</f>
         <v>7322</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="9">
         <f>F9-F10</f>
         <v>5992</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="9">
         <f>G9-G10</f>
         <v>9504</v>
       </c>
-      <c r="H11" s="7">
+      <c r="H11" s="9">
         <f>H9-H10</f>
         <v>15526</v>
       </c>
-      <c r="I11" s="7">
+      <c r="I11" s="9">
         <f>I9-I10</f>
         <v>19302</v>
       </c>
-      <c r="J11" s="7">
+      <c r="J11" s="9">
         <f>J9-J10</f>
         <v>22062</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" t="s">
-        <v>57</v>
-      </c>
-      <c r="C12" s="3">
+        <v>67</v>
+      </c>
+      <c r="C12" s="5">
         <f>C11-C13</f>
         <v>1347</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="9">
         <f>D11-D13</f>
         <v>2184</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="9">
         <f>E11-E13</f>
         <v>2058</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="9">
         <f>F11-F13</f>
         <v>1572</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G12" s="9">
         <f>G11-G13</f>
         <v>2476</v>
       </c>
-      <c r="H12" s="7">
+      <c r="H12" s="9">
         <f>H11-H13</f>
         <v>4018</v>
       </c>
-      <c r="I12" s="7">
+      <c r="I12" s="9">
         <f>I11-I13</f>
         <v>4851</v>
       </c>
-      <c r="J12" s="7">
+      <c r="J12" s="9">
         <f>J11-J13</f>
         <v>5283</v>
       </c>
     </row>
-    <row r="13" s="4" customFormat="1">
-      <c r="B13" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C13" s="5">
+    <row r="13" s="6" customFormat="1">
+      <c r="B13" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="7">
         <v>2496</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="7">
         <v>3995</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="7">
         <v>5264</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="7">
         <v>4420</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G13" s="7">
         <v>7028</v>
       </c>
-      <c r="H13" s="5">
+      <c r="H13" s="7">
         <v>11508</v>
       </c>
-      <c r="I13" s="5">
+      <c r="I13" s="7">
         <v>14451</v>
       </c>
-      <c r="J13" s="5">
+      <c r="J13" s="7">
         <v>16779</v>
       </c>
     </row>
     <row r="14"/>
     <row r="17">
       <c r="B17" t="s">
-        <v>59</v>
-      </c>
-      <c r="D17" s="8">
+        <v>69</v>
+      </c>
+      <c r="D17" s="10">
         <f>D13/C13-1</f>
         <v>0.60056089743589736</v>
       </c>
-      <c r="E17" s="8">
+      <c r="E17" s="10">
         <f>E13/D13-1</f>
         <v>0.31764705882352939</v>
       </c>
-      <c r="F17" s="8">
+      <c r="F17" s="10">
         <f>F13/E13-1</f>
         <v>-0.16033434650455924</v>
       </c>
-      <c r="G17" s="8">
+      <c r="G17" s="10">
         <f>G13/F13-1</f>
         <v>0.59004524886877818</v>
       </c>
-      <c r="H17" s="8">
+      <c r="H17" s="10">
         <f>H13/G13-1</f>
         <v>0.63745019920318735</v>
       </c>
-      <c r="I17" s="8">
+      <c r="I17" s="10">
         <f>I13/H13-1</f>
         <v>0.25573514077163706</v>
       </c>
-      <c r="J17" s="8">
+      <c r="J17" s="10">
         <f>J13/I13-1</f>
         <v>0.1610961179157151</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" t="s">
-        <v>60</v>
-      </c>
-      <c r="D18" s="8">
+        <v>70</v>
+      </c>
+      <c r="D18" s="10">
         <f>D12/C12-1</f>
         <v>0.6213808463251671</v>
       </c>
-      <c r="E18" s="8">
+      <c r="E18" s="10">
         <f>E12/D12-1</f>
         <v>-0.057692307692307709</v>
       </c>
-      <c r="F18" s="8">
+      <c r="F18" s="10">
         <f>F12/E12-1</f>
         <v>-0.23615160349854225</v>
       </c>
-      <c r="G18" s="8">
+      <c r="G18" s="10">
         <f>G12/F12-1</f>
         <v>0.57506361323155208</v>
       </c>
-      <c r="H18" s="8">
+      <c r="H18" s="10">
         <f>H12/G12-1</f>
         <v>0.62277867528271402</v>
       </c>
-      <c r="I18" s="8">
+      <c r="I18" s="10">
         <f>I12/H12-1</f>
         <v>0.20731707317073167</v>
       </c>
-      <c r="J18" s="8">
+      <c r="J18" s="10">
         <f>J12/I12-1</f>
         <v>0.089053803339517623</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" t="s">
-        <v>61</v>
-      </c>
-      <c r="D19" s="8">
+        <v>71</v>
+      </c>
+      <c r="D19" s="10">
         <f>D6/C6-1</f>
         <v>0.43541395752058953</v>
       </c>
-      <c r="E19" s="8">
+      <c r="E19" s="10">
         <f>E6/D6-1</f>
         <v>0.43031858674316781</v>
       </c>
-      <c r="F19" s="8">
+      <c r="F19" s="10">
         <f>F6/E6-1</f>
         <v>-0.0062282275942151522</v>
       </c>
-      <c r="G19" s="8">
+      <c r="G19" s="10">
         <f>G6/F6-1</f>
         <v>0.036116422349691923</v>
       </c>
-      <c r="H19" s="8">
+      <c r="H19" s="10">
         <f>H6/G6-1</f>
         <v>0.2876768505228624</v>
       </c>
-      <c r="I19" s="8">
+      <c r="I19" s="10">
         <f>I6/H6-1</f>
         <v>0.49084394904458595</v>
       </c>
-      <c r="J19" s="8">
+      <c r="J19" s="10">
         <f>J6/I6-1</f>
         <v>0.32288384512683588</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" t="s">
-        <v>62</v>
-      </c>
-      <c r="D20" s="8">
+        <v>72</v>
+      </c>
+      <c r="D20" s="10">
         <f>D8/C8-1</f>
         <v>0.28348623853211019</v>
       </c>
-      <c r="E20" s="8">
+      <c r="E20" s="10">
         <f>E8/D8-1</f>
         <v>0.34905885156063854</v>
       </c>
-      <c r="F20" s="8">
+      <c r="F20" s="10">
         <f>F8/E8-1</f>
         <v>-0.062522077004592003</v>
       </c>
-      <c r="G20" s="8">
+      <c r="G20" s="10">
         <f>G8/F8-1</f>
         <v>0.42935192162773173</v>
       </c>
-      <c r="H20" s="8">
+      <c r="H20" s="10">
         <f>H8/G8-1</f>
         <v>0.3367602477922762</v>
       </c>
-      <c r="I20" s="8">
+      <c r="I20" s="10">
         <f>I8/H8-1</f>
         <v>0.21524354170774984</v>
       </c>
-      <c r="J20" s="8">
+      <c r="J20" s="10">
         <f>J8/I8-1</f>
         <v>0.2110344827586208</v>
       </c>
     </row>
     <row r="21">
       <c r="B21" t="s">
-        <v>63</v>
-      </c>
-      <c r="D21" s="8">
+        <v>73</v>
+      </c>
+      <c r="D21" s="10">
         <f>D13/D5</f>
         <v>0.21594594594594593</v>
       </c>
-      <c r="E21" s="8">
+      <c r="E21" s="10">
         <f>E13/E5</f>
         <v>0.19949973470779958</v>
       </c>
-      <c r="F21" s="8">
+      <c r="F21" s="10">
         <f>F13/F5</f>
         <v>0.16564854026908518</v>
       </c>
-      <c r="G21" s="8">
+      <c r="G21" s="10">
         <f>G13/G5</f>
         <v>0.22206774519716885</v>
       </c>
-      <c r="H21" s="8">
+      <c r="H21" s="10">
         <f>H13/H5</f>
         <v>0.27785021005359989</v>
       </c>
-      <c r="I21" s="8">
+      <c r="I21" s="10">
         <f>I13/I5</f>
         <v>0.26282669188658314</v>
       </c>
-      <c r="J21" s="8">
+      <c r="J21" s="10">
         <f>J13/J5</f>
         <v>0.24064539261384008</v>
       </c>
@@ -1950,373 +2042,373 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" style="9" width="9.140625"/>
-    <col customWidth="1" min="2" max="2" style="9" width="50.421875"/>
-    <col customWidth="1" min="3" max="3" style="9" width="24.00390625"/>
-    <col min="4" max="16384" style="9" width="9.140625"/>
+    <col min="1" max="1" style="11" width="9.140625"/>
+    <col customWidth="1" min="2" max="2" style="11" width="50.421875"/>
+    <col customWidth="1" min="3" max="3" style="11" width="24.00390625"/>
+    <col min="4" max="16384" style="11" width="9.140625"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.25">
-      <c r="B2" s="2" t="s">
-        <v>64</v>
+      <c r="B2" s="4" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="3" ht="14.25">
-      <c r="B3" s="9"/>
+      <c r="B3" s="11"/>
     </row>
     <row r="5" ht="16.5">
-      <c r="A5" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>66</v>
+      <c r="A5" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="7" ht="16.5">
-      <c r="A7" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="C7" s="11">
+      <c r="A7" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" s="13">
         <v>0.39000000000000001</v>
       </c>
     </row>
     <row r="8" ht="16.5">
-      <c r="A8" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="C8" s="12">
+      <c r="A8" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" s="14">
         <v>0.34000000000000002</v>
       </c>
     </row>
     <row r="9" ht="16.5">
-      <c r="A9" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="C9" s="12">
+      <c r="A9" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" s="14">
         <v>0.51000000000000001</v>
       </c>
     </row>
     <row r="10" ht="14.25">
-      <c r="C10" s="12"/>
+      <c r="C10" s="14"/>
     </row>
     <row r="11" ht="14.25">
-      <c r="C11" s="12"/>
+      <c r="C11" s="14"/>
     </row>
     <row r="12" ht="14.25">
-      <c r="C12" s="12"/>
+      <c r="C12" s="14"/>
     </row>
     <row r="13" ht="16.5">
-      <c r="B13" s="10" t="str">
+      <c r="B13" s="12" t="str">
         <f>B7</f>
         <v xml:space="preserve">Bajaj finserv ltd</v>
       </c>
-      <c r="C13" s="12"/>
+      <c r="C13" s="14"/>
     </row>
     <row r="14" ht="16.5">
-      <c r="A14" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="C14" s="12">
+      <c r="A14" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14" s="14">
         <v>0.51390000000000002</v>
       </c>
     </row>
     <row r="15" ht="16.5">
-      <c r="A15" s="9"/>
-      <c r="B15" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="C15" s="12">
+      <c r="A15" s="11"/>
+      <c r="B15" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C15" s="14">
         <v>0.73999999999999999</v>
       </c>
     </row>
     <row r="16" ht="16.5">
-      <c r="B16" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="C16" s="12">
+      <c r="B16" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16" s="14">
         <v>0.73999999999999999</v>
       </c>
     </row>
     <row r="17" ht="16.5">
-      <c r="B17" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="C17" s="12">
+      <c r="B17" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="C17" s="14">
         <v>0.80100000000000005</v>
       </c>
     </row>
     <row r="18" ht="16.5">
-      <c r="B18" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="C18" s="12">
+      <c r="B18" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" s="14">
         <v>1</v>
       </c>
     </row>
     <row r="19" ht="14.25">
-      <c r="C19" s="12"/>
+      <c r="C19" s="14"/>
     </row>
     <row r="20" ht="14.25">
-      <c r="C20" s="12"/>
+      <c r="C20" s="14"/>
     </row>
     <row r="21" ht="16.5">
-      <c r="B21" s="10" t="str">
+      <c r="B21" s="12" t="str">
         <f>B14</f>
         <v xml:space="preserve">Bajaj Finance Ltd</v>
       </c>
-      <c r="C21" s="12"/>
+      <c r="C21" s="14"/>
     </row>
     <row r="22" ht="16.5">
-      <c r="A22" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="C22" s="12">
+      <c r="A22" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="C22" s="14">
         <v>0.88749999999999996</v>
       </c>
     </row>
     <row r="23" ht="16.5">
-      <c r="B23" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="C23" s="12">
+      <c r="B23" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="C23" s="14">
         <v>1</v>
       </c>
     </row>
     <row r="24" ht="14.25">
-      <c r="C24" s="11"/>
+      <c r="C24" s="13"/>
     </row>
     <row r="27" ht="16.5">
-      <c r="B27" s="10" t="s">
-        <v>78</v>
+      <c r="B27" s="12" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="29" ht="16.5">
-      <c r="B29" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="C29" s="13">
+      <c r="B29" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="C29" s="15">
         <v>49500</v>
       </c>
     </row>
     <row r="30" ht="16.5">
-      <c r="A30" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="C30" s="13">
+      <c r="A30" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="C30" s="15">
         <v>62700</v>
       </c>
     </row>
     <row r="31" ht="16.5">
-      <c r="B31" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="C31" s="13">
+      <c r="B31" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="C31" s="15">
         <v>46250</v>
       </c>
     </row>
     <row r="32" ht="16.5">
-      <c r="B32" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="C32" s="13">
+      <c r="B32" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="C32" s="15">
         <v>21250</v>
       </c>
     </row>
     <row r="33" ht="16.5">
-      <c r="B33" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="C33" s="13">
+      <c r="B33" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="C33" s="15">
         <v>30700</v>
       </c>
     </row>
     <row r="34" ht="16.5">
-      <c r="B34" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="C34" s="13">
+      <c r="B34" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="C34" s="15">
         <v>550</v>
       </c>
     </row>
     <row r="35" ht="16.5">
-      <c r="B35" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="C35" s="13">
+      <c r="B35" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="C35" s="15">
         <v>8900</v>
       </c>
     </row>
     <row r="36" ht="16.5">
-      <c r="B36" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="C36" s="13">
+      <c r="B36" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="C36" s="15">
         <v>2300</v>
       </c>
     </row>
     <row r="37" ht="16.5">
-      <c r="B37" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="C37" s="13">
+      <c r="B37" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="C37" s="15">
         <v>100</v>
       </c>
     </row>
     <row r="38" ht="16.5">
-      <c r="B38" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="C38" s="13">
+      <c r="B38" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C38" s="15">
         <v>850</v>
       </c>
     </row>
     <row r="39" ht="16.5">
-      <c r="B39" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="C39" s="13">
+      <c r="B39" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C39" s="15">
         <v>9200</v>
       </c>
     </row>
     <row r="40" ht="16.5">
-      <c r="B40" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="C40" s="13">
+      <c r="B40" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="C40" s="15">
         <v>232200</v>
       </c>
     </row>
     <row r="41" ht="16.5">
-      <c r="B41" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="C41" s="13">
+      <c r="B41" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="C41" s="15">
         <v>7500</v>
       </c>
     </row>
     <row r="44" ht="16.5">
-      <c r="B44" s="10" t="s">
-        <v>93</v>
+      <c r="B44" s="12" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="45" ht="16.5">
-      <c r="B45" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="C45" s="13">
+      <c r="B45" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="C45" s="15">
         <v>17319</v>
       </c>
     </row>
     <row r="46" ht="16.5">
-      <c r="B46" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="C46" s="13">
+      <c r="B46" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="C46" s="15">
         <v>29109</v>
       </c>
     </row>
     <row r="47" ht="16.5">
-      <c r="B47" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="C47" s="13">
+      <c r="B47" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="C47" s="15">
         <v>87696</v>
       </c>
     </row>
     <row r="48" ht="16.5">
-      <c r="B48" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="C48" s="13">
+      <c r="B48" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="C48" s="15">
         <v>7944</v>
       </c>
     </row>
     <row r="49" ht="16.5">
-      <c r="A49" s="9"/>
-      <c r="B49" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="C49" s="13">
+      <c r="A49" s="11"/>
+      <c r="B49" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="C49" s="15">
         <v>21467</v>
       </c>
     </row>
     <row r="50" ht="16.5">
-      <c r="B50" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="C50" s="13">
+      <c r="B50" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="C50" s="15">
         <v>8307</v>
       </c>
     </row>
     <row r="51" ht="16.5">
-      <c r="B51" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="C51" s="13">
+      <c r="B51" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C51" s="15">
         <v>50345</v>
       </c>
     </row>
     <row r="52" ht="16.5">
-      <c r="B52" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="C52" s="13">
+      <c r="B52" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="C52" s="15">
         <v>11876</v>
       </c>
     </row>
     <row r="53" ht="16.5">
-      <c r="B53" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="C53" s="13">
+      <c r="B53" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="C53" s="15">
         <v>27760</v>
       </c>
     </row>
     <row r="54" ht="16.5">
-      <c r="B54" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="C54" s="13">
+      <c r="B54" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="C54" s="15">
         <v>25377</v>
       </c>
     </row>
     <row r="55" ht="16.5">
-      <c r="B55" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="C55" s="13">
+      <c r="B55" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="C55" s="15">
         <v>129461</v>
       </c>
     </row>
     <row r="56" ht="16.5">
-      <c r="B56" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="C56" s="14">
+      <c r="B56" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="C56" s="16">
         <f>SUM(C45:C55)</f>
         <v>416661</v>
       </c>
     </row>
     <row r="57" ht="16.5">
-      <c r="B57" s="9"/>
+      <c r="B57" s="11"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2347,191 +2439,191 @@
   <sheetData>
     <row r="1" ht="14.25">
       <c r="A1" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" ht="14.25"/>
     <row r="3" ht="14.25">
-      <c r="C3" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>44</v>
+      <c r="C3" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="4" ht="14.25">
       <c r="B4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C4" s="3">
+        <v>61</v>
+      </c>
+      <c r="C4" s="5">
         <v>4410</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="5">
         <v>6296</v>
       </c>
     </row>
     <row r="5" ht="14.25">
       <c r="B5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C5" s="3">
+        <v>117</v>
+      </c>
+      <c r="C5" s="5">
         <v>1417</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="5">
         <v>1957</v>
       </c>
     </row>
-    <row r="6" s="4" customFormat="1" ht="14.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
+    <row r="6" s="6" customFormat="1" ht="14.25">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
     </row>
     <row r="7" ht="14.25">
       <c r="A7" t="s">
-        <v>108</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="C7" s="5">
+        <v>118</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C7" s="7">
         <f>C4-C5</f>
         <v>2993</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="7">
         <f>D4-D5</f>
         <v>4339</v>
       </c>
     </row>
     <row r="8" ht="14.25">
       <c r="B8" t="s">
-        <v>110</v>
-      </c>
-      <c r="C8" s="3">
+        <v>120</v>
+      </c>
+      <c r="C8" s="5">
         <v>903</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="5">
         <v>1352</v>
       </c>
     </row>
     <row r="9" ht="14.25">
-      <c r="B9" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="C9" s="5">
+      <c r="B9" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C9" s="7">
         <f>C4-C5-C8</f>
         <v>2090</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="7">
         <f>D4-D5-D8</f>
         <v>2987</v>
       </c>
     </row>
     <row r="10" ht="14.25">
       <c r="B10" t="s">
-        <v>57</v>
-      </c>
-      <c r="C10" s="3">
+        <v>67</v>
+      </c>
+      <c r="C10" s="5">
         <v>536</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="5">
         <v>766</v>
       </c>
     </row>
     <row r="11" ht="14.25">
-      <c r="B11" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C11" s="5">
+      <c r="B11" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="7">
         <f>C9-C10</f>
         <v>1554</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="7">
         <f>D9-D10</f>
         <v>2221</v>
       </c>
     </row>
     <row r="12" ht="14.25">
       <c r="B12" t="s">
-        <v>112</v>
-      </c>
-      <c r="C12" s="3">
+        <v>122</v>
+      </c>
+      <c r="C12" s="5">
         <v>11426</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="5">
         <v>15224</v>
       </c>
     </row>
     <row r="13" ht="14.25">
       <c r="B13" t="s">
-        <v>113</v>
-      </c>
-      <c r="C13" s="3">
+        <v>123</v>
+      </c>
+      <c r="C13" s="5">
         <v>70771</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="5">
         <v>92292</v>
       </c>
     </row>
     <row r="14" ht="14.25"/>
     <row r="15" ht="14.25">
       <c r="B15" t="s">
-        <v>114</v>
-      </c>
-      <c r="C15" s="8">
+        <v>124</v>
+      </c>
+      <c r="C15" s="10">
         <f>C11/C12</f>
         <v>0.13600560126028358</v>
       </c>
-      <c r="D15" s="16">
+      <c r="D15" s="17">
         <f>D11/D12</f>
         <v>0.14588807146610616</v>
       </c>
     </row>
     <row r="16" ht="14.25">
       <c r="B16" t="s">
-        <v>115</v>
-      </c>
-      <c r="C16" s="17">
+        <v>125</v>
+      </c>
+      <c r="C16" s="18">
         <f>C13/C12</f>
         <v>6.1938561176264662</v>
       </c>
-      <c r="D16" s="18">
+      <c r="D16" s="19">
         <f>D13/D12</f>
         <v>6.0622700998423538</v>
       </c>
     </row>
     <row r="17" ht="14.25">
       <c r="B17" t="s">
-        <v>116</v>
-      </c>
-      <c r="C17" s="8">
+        <v>126</v>
+      </c>
+      <c r="C17" s="10">
         <f>C5/C4</f>
         <v>0.32131519274376419</v>
       </c>
-      <c r="D17" s="16">
+      <c r="D17" s="17">
         <f>D5/D4</f>
         <v>0.31083227445997458</v>
       </c>
     </row>
     <row r="18" ht="14.25">
       <c r="B18" t="s">
-        <v>117</v>
-      </c>
-      <c r="C18" s="8">
+        <v>127</v>
+      </c>
+      <c r="C18" s="10">
         <f>C8/C7</f>
         <v>0.30170397594386905</v>
       </c>
-      <c r="D18" s="16">
+      <c r="D18" s="17">
         <f>D8/D7</f>
         <v>0.3115925328416686</v>
       </c>
     </row>
     <row r="19" ht="14.25">
       <c r="A19" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="B19" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -2551,241 +2643,240 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" style="9" width="9.140625"/>
-    <col customWidth="1" min="2" max="2" style="9" width="46.8515625"/>
-    <col min="3" max="3" style="9" width="9.140625"/>
-    <col min="4" max="16384" style="9" width="9.140625"/>
+    <col min="1" max="1" style="11" width="9.140625"/>
+    <col customWidth="1" min="2" max="2" style="11" width="46.8515625"/>
+    <col min="3" max="16384" style="11" width="9.140625"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5">
-      <c r="A1" s="19"/>
-      <c r="B1" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
+      <c r="A1" s="20"/>
+      <c r="B1" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
     </row>
     <row r="2">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
     </row>
     <row r="3" ht="15">
-      <c r="A3" s="19"/>
-      <c r="B3" s="22" t="s">
-        <v>121</v>
-      </c>
-      <c r="C3" s="23" t="s">
-        <v>122</v>
-      </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
+      <c r="A3" s="20"/>
+      <c r="B3" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
     </row>
     <row r="4" ht="15">
-      <c r="A4" s="24" t="s">
-        <v>123</v>
-      </c>
-      <c r="B4" s="24" t="s">
-        <v>124</v>
-      </c>
-      <c r="C4" s="25">
+      <c r="A4" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="C4" s="26">
         <v>52.700000000000003</v>
       </c>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
     </row>
     <row r="5" ht="15">
-      <c r="A5" s="19"/>
-      <c r="B5" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="C5" s="25">
+      <c r="A5" s="20"/>
+      <c r="B5" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="C5" s="26">
         <v>16.300000000000001</v>
       </c>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
     </row>
     <row r="6" ht="15">
-      <c r="A6" s="19"/>
-      <c r="B6" s="24" t="s">
-        <v>126</v>
-      </c>
-      <c r="C6" s="25">
+      <c r="A6" s="20"/>
+      <c r="B6" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="C6" s="26">
         <v>31</v>
       </c>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
     </row>
     <row r="7">
-      <c r="A7" s="19"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
+      <c r="A7" s="20"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
     </row>
     <row r="8">
-      <c r="A8" s="19"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
+      <c r="A8" s="20"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
     </row>
     <row r="9" ht="15">
-      <c r="A9" s="19"/>
-      <c r="B9" s="22" t="s">
-        <v>127</v>
-      </c>
-      <c r="C9" s="24" t="s">
-        <v>128</v>
-      </c>
-      <c r="D9" s="24" t="s">
-        <v>129</v>
-      </c>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
+      <c r="A9" s="20"/>
+      <c r="B9" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>138</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
     </row>
     <row r="10" ht="15">
-      <c r="A10" s="19"/>
-      <c r="B10" s="24" t="s">
-        <v>130</v>
-      </c>
-      <c r="C10" s="25">
+      <c r="A10" s="20"/>
+      <c r="B10" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="C10" s="26">
         <v>100</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="D10" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
     </row>
     <row r="11" ht="15">
-      <c r="A11" s="19"/>
-      <c r="B11" s="24" t="s">
-        <v>131</v>
-      </c>
-      <c r="C11" s="25">
+      <c r="A11" s="20"/>
+      <c r="B11" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="C11" s="26">
         <v>100</v>
       </c>
-      <c r="D11" s="23" t="s">
-        <v>132</v>
-      </c>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
+      <c r="D11" s="24" t="s">
+        <v>142</v>
+      </c>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
     </row>
     <row r="12" ht="15">
-      <c r="A12" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="B12" s="24" t="s">
-        <v>133</v>
-      </c>
-      <c r="C12" s="25">
+      <c r="A12" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="B12" s="25" t="s">
+        <v>143</v>
+      </c>
+      <c r="C12" s="26">
         <v>74</v>
       </c>
-      <c r="D12" s="23" t="s">
-        <v>134</v>
-      </c>
-      <c r="E12" s="21"/>
-      <c r="F12" s="19"/>
+      <c r="D12" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="E12" s="22"/>
+      <c r="F12" s="20"/>
     </row>
     <row r="13" ht="15">
-      <c r="A13" s="19"/>
-      <c r="B13" s="24" t="s">
-        <v>135</v>
-      </c>
-      <c r="C13" s="25">
+      <c r="A13" s="20"/>
+      <c r="B13" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="C13" s="26">
         <v>50</v>
       </c>
-      <c r="D13" s="23" t="s">
-        <v>136</v>
-      </c>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
+      <c r="D13" s="24" t="s">
+        <v>146</v>
+      </c>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
     </row>
     <row r="14" ht="15">
-      <c r="A14" s="19"/>
-      <c r="B14" s="24" t="s">
-        <v>137</v>
-      </c>
-      <c r="C14" s="25">
+      <c r="A14" s="20"/>
+      <c r="B14" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="C14" s="26">
         <v>51</v>
       </c>
-      <c r="D14" s="23" t="s">
-        <v>138</v>
-      </c>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
+      <c r="D14" s="24" t="s">
+        <v>148</v>
+      </c>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
     </row>
     <row r="15" ht="15">
-      <c r="A15" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="B15" s="24" t="s">
-        <v>139</v>
-      </c>
-      <c r="C15" s="25">
+      <c r="A15" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="C15" s="26">
         <v>45</v>
       </c>
-      <c r="D15" s="23" t="s">
-        <v>140</v>
-      </c>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
+      <c r="D15" s="24" t="s">
+        <v>150</v>
+      </c>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
     </row>
     <row r="16" ht="15">
-      <c r="A16" s="19"/>
-      <c r="B16" s="24" t="s">
-        <v>141</v>
-      </c>
-      <c r="C16" s="25">
+      <c r="A16" s="20"/>
+      <c r="B16" s="25" t="s">
+        <v>151</v>
+      </c>
+      <c r="C16" s="26">
         <v>46</v>
       </c>
-      <c r="D16" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="E16" s="21"/>
-      <c r="F16" s="19"/>
+      <c r="D16" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="E16" s="22"/>
+      <c r="F16" s="20"/>
     </row>
     <row r="17" ht="15">
-      <c r="A17" s="19"/>
-      <c r="B17" s="24" t="s">
-        <v>143</v>
-      </c>
-      <c r="C17" s="25">
+      <c r="A17" s="20"/>
+      <c r="B17" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="C17" s="26">
         <v>100</v>
       </c>
-      <c r="D17" s="23" t="s">
-        <v>144</v>
-      </c>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
+      <c r="D17" s="24" t="s">
+        <v>154</v>
+      </c>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
     </row>
     <row r="18">
-      <c r="A18" s="19"/>
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
+      <c r="A18" s="20"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
     </row>
     <row r="19">
-      <c r="A19" s="19"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
+      <c r="A19" s="20"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>